<commit_message>
Added set 14 and some of its results
</commit_message>
<xml_diff>
--- a/Tests/Set 13 [New Code - Best Effort VS Reliable]/100,000,000 Iteration + 100,000 Latency Count/Reliable Multicast/Reliable Multicast Test Summary.xlsx
+++ b/Tests/Set 13 [New Code - Best Effort VS Reliable]/100,000,000 Iteration + 100,000 Latency Count/Reliable Multicast/Reliable Multicast Test Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalee\Documents\Performance-Testing\Tests\Set 13 [New Code - Best Effort VS Reliable]\100,000,000 Iteration + 100,000 Latency Count\Reliable Multicast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FE887F-E74C-4E21-8475-646BF5AFACAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738735E1-152A-46D7-92AF-98AB226A1CD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -892,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>